<commit_message>
Complete syntax analyzer test
what we should do will implement  error checking and if error is detected, we make error message about what kind of error is this
</commit_message>
<xml_diff>
--- a/bin/Docs/SLRTable.xlsx
+++ b/bin/Docs/SLRTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YoungJae\Desktop\컴파일러\project2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YoungJae\eclipse-workspace\syntax_analyzer\src\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0047D1-D8F1-47C2-9AAF-010FF4EBD8C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD8F9C2-08AA-4DDF-AEB3-1087A23C3269}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E5975004-6C18-49A2-8386-EB4D73A3595F}"/>
+    <workbookView xWindow="-6945" yWindow="7170" windowWidth="14400" windowHeight="11010" xr2:uid="{E5975004-6C18-49A2-8386-EB4D73A3595F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="100">
   <si>
     <t>vtype</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -422,6 +422,14 @@
   </si>
   <si>
     <t>S13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S33</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -951,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70100367-4A23-4B04-87CE-99CE78C24379}">
   <dimension ref="A1:AF72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1932,9 +1940,13 @@
       <c r="E24" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="8"/>
+      <c r="F24" s="8" t="s">
+        <v>98</v>
+      </c>
       <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
+      <c r="H24" s="8" t="s">
+        <v>99</v>
+      </c>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>

</xml_diff>